<commit_message>
add require choose partner, get data
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Invoice no. / Credit no.</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>{VATVoucher}</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>{IssueDate}</t>
@@ -149,6 +146,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -231,6 +231,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +711,7 @@
     <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -748,7 +758,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -772,10 +782,10 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>20</v>
@@ -795,7 +805,7 @@
       <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -804,18 +814,16 @@
       <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="Q2" s="3"/>
       <c r="R2" s="6" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
reformat balance's value, fix get
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
@@ -692,9 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
change get data report Agency
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intern.lth012\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17805" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Invoice no. / Credit no.</t>
   </si>
@@ -91,12 +91,21 @@
     <t>VAT no. / ID voucher</t>
   </si>
   <si>
+    <t>SOA/SM</t>
+  </si>
+  <si>
     <t>{INVCreNo}</t>
   </si>
   <si>
     <t>{JobNo}</t>
   </si>
   <si>
+    <t>{Type}</t>
+  </si>
+  <si>
+    <t>{IssueDate}</t>
+  </si>
+  <si>
     <t>{FlexId}</t>
   </si>
   <si>
@@ -127,28 +136,22 @@
     <t>{Balance}</t>
   </si>
   <si>
+    <t>{InvDueDay}</t>
+  </si>
+  <si>
     <t>{Status}</t>
   </si>
   <si>
     <t>{VATVoucher}</t>
   </si>
   <si>
-    <t>{IssueDate}</t>
-  </si>
-  <si>
-    <t>{Type}</t>
-  </si>
-  <si>
-    <t>{InvDueDay}</t>
+    <t>{SoaSm}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -214,33 +217,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,18 +686,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection sqref="A1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -711,14 +707,14 @@
     <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +724,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -758,7 +754,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -770,62 +766,68 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="6" t="s">
-        <v>31</v>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change condition in get data
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intern.lth012\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -688,9 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
error handling, update template
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/FlexportnewSOAtemplate.xlsx
@@ -688,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -699,13 +699,13 @@
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>

</xml_diff>